<commit_message>
[QSI & QUI] Bug 13018
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者氏名変更届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者氏名変更届_帳票テンプレート.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6445611F-D027-438C-A97C-CF5AAF5864B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="被保険者氏名変更（訂正）届 " sheetId="1" r:id="rId1"/>
@@ -493,7 +492,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22">
     <font>
       <sz val="11"/>
@@ -635,7 +634,7 @@
     </font>
     <font>
       <b/>
-      <sz val="8.5"/>
+      <sz val="8"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -1529,6 +1528,471 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1559,475 +2023,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4173,12 +4172,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AM37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+      <selection activeCell="K23" sqref="K23:S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4317,26 +4316,26 @@
       <c r="V3" s="9"/>
       <c r="W3" s="9"/>
       <c r="X3" s="1"/>
-      <c r="Y3" s="136" t="s">
+      <c r="Y3" s="182" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="137"/>
-      <c r="AA3" s="138"/>
-      <c r="AB3" s="136" t="s">
+      <c r="Z3" s="183"/>
+      <c r="AA3" s="184"/>
+      <c r="AB3" s="182" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="137"/>
-      <c r="AD3" s="138"/>
-      <c r="AE3" s="136" t="s">
+      <c r="AC3" s="183"/>
+      <c r="AD3" s="184"/>
+      <c r="AE3" s="182" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="137"/>
-      <c r="AG3" s="138"/>
-      <c r="AH3" s="136" t="s">
+      <c r="AF3" s="183"/>
+      <c r="AG3" s="184"/>
+      <c r="AH3" s="182" t="s">
         <v>20</v>
       </c>
-      <c r="AI3" s="137"/>
-      <c r="AJ3" s="138"/>
+      <c r="AI3" s="183"/>
+      <c r="AJ3" s="184"/>
       <c r="AK3" s="10"/>
       <c r="AL3" s="11"/>
     </row>
@@ -4365,24 +4364,24 @@
       <c r="V4" s="9"/>
       <c r="W4" s="9"/>
       <c r="X4" s="1"/>
-      <c r="Y4" s="139" t="s">
+      <c r="Y4" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="Z4" s="140"/>
-      <c r="AA4" s="141"/>
-      <c r="AB4" s="139" t="s">
+      <c r="Z4" s="180"/>
+      <c r="AA4" s="181"/>
+      <c r="AB4" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="AC4" s="140"/>
-      <c r="AD4" s="141"/>
-      <c r="AE4" s="139" t="s">
+      <c r="AC4" s="180"/>
+      <c r="AD4" s="181"/>
+      <c r="AE4" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="AF4" s="140"/>
-      <c r="AG4" s="141"/>
-      <c r="AH4" s="139"/>
-      <c r="AI4" s="140"/>
-      <c r="AJ4" s="141"/>
+      <c r="AF4" s="180"/>
+      <c r="AG4" s="181"/>
+      <c r="AH4" s="179"/>
+      <c r="AI4" s="180"/>
+      <c r="AJ4" s="181"/>
       <c r="AK4" s="10"/>
       <c r="AL4" s="11"/>
     </row>
@@ -4396,39 +4395,39 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="106" t="s">
+      <c r="K5" s="217"/>
+      <c r="L5" s="217"/>
+      <c r="M5" s="221" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
+      <c r="N5" s="221"/>
+      <c r="O5" s="221"/>
+      <c r="P5" s="221"/>
+      <c r="Q5" s="221"/>
+      <c r="R5" s="221"/>
+      <c r="S5" s="221"/>
+      <c r="T5" s="221"/>
+      <c r="U5" s="221"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
-      <c r="Y5" s="127"/>
-      <c r="Z5" s="128"/>
-      <c r="AA5" s="129"/>
-      <c r="AB5" s="127"/>
-      <c r="AC5" s="128"/>
-      <c r="AD5" s="129"/>
-      <c r="AE5" s="127"/>
-      <c r="AF5" s="128"/>
-      <c r="AG5" s="129"/>
-      <c r="AH5" s="127"/>
-      <c r="AI5" s="128"/>
-      <c r="AJ5" s="129"/>
+      <c r="Y5" s="175"/>
+      <c r="Z5" s="176"/>
+      <c r="AA5" s="177"/>
+      <c r="AB5" s="175"/>
+      <c r="AC5" s="176"/>
+      <c r="AD5" s="177"/>
+      <c r="AE5" s="175"/>
+      <c r="AF5" s="176"/>
+      <c r="AG5" s="177"/>
+      <c r="AH5" s="175"/>
+      <c r="AI5" s="176"/>
+      <c r="AJ5" s="177"/>
       <c r="AK5" s="13"/>
-      <c r="AL5" s="167"/>
+      <c r="AL5" s="188"/>
     </row>
     <row r="6" spans="1:39" ht="27.75" customHeight="1">
       <c r="A6" s="1"/>
@@ -4440,37 +4439,37 @@
       <c r="G6" s="1"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
-      <c r="J6" s="133" t="s">
+      <c r="J6" s="238" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="133"/>
-      <c r="L6" s="133"/>
-      <c r="M6" s="106"/>
-      <c r="N6" s="106"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="106"/>
-      <c r="U6" s="106"/>
+      <c r="K6" s="238"/>
+      <c r="L6" s="238"/>
+      <c r="M6" s="221"/>
+      <c r="N6" s="221"/>
+      <c r="O6" s="221"/>
+      <c r="P6" s="221"/>
+      <c r="Q6" s="221"/>
+      <c r="R6" s="221"/>
+      <c r="S6" s="221"/>
+      <c r="T6" s="221"/>
+      <c r="U6" s="221"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
-      <c r="Y6" s="130"/>
-      <c r="Z6" s="131"/>
-      <c r="AA6" s="132"/>
-      <c r="AB6" s="130"/>
-      <c r="AC6" s="131"/>
-      <c r="AD6" s="132"/>
-      <c r="AE6" s="130"/>
-      <c r="AF6" s="131"/>
-      <c r="AG6" s="132"/>
-      <c r="AH6" s="130"/>
-      <c r="AI6" s="131"/>
-      <c r="AJ6" s="132"/>
+      <c r="Y6" s="193"/>
+      <c r="Z6" s="108"/>
+      <c r="AA6" s="109"/>
+      <c r="AB6" s="193"/>
+      <c r="AC6" s="108"/>
+      <c r="AD6" s="109"/>
+      <c r="AE6" s="193"/>
+      <c r="AF6" s="108"/>
+      <c r="AG6" s="109"/>
+      <c r="AH6" s="193"/>
+      <c r="AI6" s="108"/>
+      <c r="AJ6" s="109"/>
       <c r="AK6" s="13"/>
-      <c r="AL6" s="167"/>
+      <c r="AL6" s="188"/>
     </row>
     <row r="7" spans="1:39" ht="35.25" customHeight="1">
       <c r="A7" s="1"/>
@@ -4515,155 +4514,155 @@
     <row r="8" spans="1:39" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="96" t="s">
+      <c r="C8" s="216" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="142" t="s">
+      <c r="D8" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="127" t="s">
+      <c r="E8" s="175" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="128"/>
-      <c r="G8" s="128"/>
-      <c r="H8" s="128"/>
-      <c r="I8" s="128"/>
-      <c r="J8" s="129"/>
-      <c r="K8" s="127" t="s">
+      <c r="F8" s="176"/>
+      <c r="G8" s="176"/>
+      <c r="H8" s="176"/>
+      <c r="I8" s="176"/>
+      <c r="J8" s="177"/>
+      <c r="K8" s="175" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="128"/>
-      <c r="M8" s="129"/>
-      <c r="N8" s="127" t="s">
+      <c r="L8" s="176"/>
+      <c r="M8" s="177"/>
+      <c r="N8" s="175" t="s">
         <v>27</v>
       </c>
-      <c r="O8" s="128"/>
-      <c r="P8" s="128"/>
-      <c r="Q8" s="128"/>
-      <c r="R8" s="128"/>
-      <c r="S8" s="128"/>
-      <c r="T8" s="128"/>
-      <c r="U8" s="128"/>
-      <c r="V8" s="128"/>
-      <c r="W8" s="128"/>
-      <c r="X8" s="128"/>
-      <c r="Y8" s="129"/>
-      <c r="Z8" s="127" t="s">
+      <c r="O8" s="176"/>
+      <c r="P8" s="176"/>
+      <c r="Q8" s="176"/>
+      <c r="R8" s="176"/>
+      <c r="S8" s="176"/>
+      <c r="T8" s="176"/>
+      <c r="U8" s="176"/>
+      <c r="V8" s="176"/>
+      <c r="W8" s="176"/>
+      <c r="X8" s="176"/>
+      <c r="Y8" s="177"/>
+      <c r="Z8" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="AA8" s="128"/>
-      <c r="AB8" s="128"/>
-      <c r="AC8" s="128"/>
-      <c r="AD8" s="128"/>
-      <c r="AE8" s="128"/>
-      <c r="AF8" s="128"/>
-      <c r="AG8" s="129"/>
-      <c r="AH8" s="172" t="s">
+      <c r="AA8" s="176"/>
+      <c r="AB8" s="176"/>
+      <c r="AC8" s="176"/>
+      <c r="AD8" s="176"/>
+      <c r="AE8" s="176"/>
+      <c r="AF8" s="176"/>
+      <c r="AG8" s="177"/>
+      <c r="AH8" s="194" t="s">
         <v>30</v>
       </c>
-      <c r="AI8" s="173"/>
-      <c r="AJ8" s="152"/>
+      <c r="AI8" s="195"/>
+      <c r="AJ8" s="208"/>
       <c r="AK8" s="15"/>
       <c r="AL8" s="16"/>
     </row>
     <row r="9" spans="1:39">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="142"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="103"/>
-      <c r="L9" s="104"/>
-      <c r="M9" s="105"/>
-      <c r="N9" s="103"/>
-      <c r="O9" s="104"/>
-      <c r="P9" s="104"/>
-      <c r="Q9" s="104"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
-      <c r="T9" s="104"/>
-      <c r="U9" s="104"/>
-      <c r="V9" s="104"/>
-      <c r="W9" s="104"/>
-      <c r="X9" s="104"/>
-      <c r="Y9" s="105"/>
-      <c r="Z9" s="103"/>
-      <c r="AA9" s="104"/>
-      <c r="AB9" s="104"/>
-      <c r="AC9" s="104"/>
-      <c r="AD9" s="104"/>
-      <c r="AE9" s="104"/>
-      <c r="AF9" s="104"/>
-      <c r="AG9" s="105"/>
-      <c r="AH9" s="168" t="s">
+      <c r="C9" s="216"/>
+      <c r="D9" s="199"/>
+      <c r="E9" s="178"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="178"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="106"/>
+      <c r="N9" s="178"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="105"/>
+      <c r="Q9" s="105"/>
+      <c r="R9" s="105"/>
+      <c r="S9" s="105"/>
+      <c r="T9" s="105"/>
+      <c r="U9" s="105"/>
+      <c r="V9" s="105"/>
+      <c r="W9" s="105"/>
+      <c r="X9" s="105"/>
+      <c r="Y9" s="106"/>
+      <c r="Z9" s="178"/>
+      <c r="AA9" s="105"/>
+      <c r="AB9" s="105"/>
+      <c r="AC9" s="105"/>
+      <c r="AD9" s="105"/>
+      <c r="AE9" s="105"/>
+      <c r="AF9" s="105"/>
+      <c r="AG9" s="106"/>
+      <c r="AH9" s="189" t="s">
         <v>31</v>
       </c>
-      <c r="AI9" s="169"/>
-      <c r="AJ9" s="153"/>
+      <c r="AI9" s="190"/>
+      <c r="AJ9" s="209"/>
       <c r="AK9" s="15"/>
       <c r="AL9" s="16"/>
     </row>
     <row r="10" spans="1:39" ht="14.25" thickBot="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="142"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="105"/>
-      <c r="K10" s="155"/>
-      <c r="L10" s="156"/>
-      <c r="M10" s="157"/>
-      <c r="N10" s="155"/>
-      <c r="O10" s="156"/>
-      <c r="P10" s="156"/>
-      <c r="Q10" s="156"/>
-      <c r="R10" s="156"/>
-      <c r="S10" s="156"/>
-      <c r="T10" s="156"/>
-      <c r="U10" s="156"/>
-      <c r="V10" s="156"/>
-      <c r="W10" s="156"/>
-      <c r="X10" s="156"/>
-      <c r="Y10" s="157"/>
-      <c r="Z10" s="155"/>
-      <c r="AA10" s="156"/>
-      <c r="AB10" s="156"/>
-      <c r="AC10" s="156"/>
-      <c r="AD10" s="156"/>
-      <c r="AE10" s="156"/>
-      <c r="AF10" s="156"/>
-      <c r="AG10" s="157"/>
-      <c r="AH10" s="170" t="s">
+      <c r="C10" s="216"/>
+      <c r="D10" s="199"/>
+      <c r="E10" s="178"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="106"/>
+      <c r="K10" s="196"/>
+      <c r="L10" s="197"/>
+      <c r="M10" s="198"/>
+      <c r="N10" s="196"/>
+      <c r="O10" s="197"/>
+      <c r="P10" s="197"/>
+      <c r="Q10" s="197"/>
+      <c r="R10" s="197"/>
+      <c r="S10" s="197"/>
+      <c r="T10" s="197"/>
+      <c r="U10" s="197"/>
+      <c r="V10" s="197"/>
+      <c r="W10" s="197"/>
+      <c r="X10" s="197"/>
+      <c r="Y10" s="198"/>
+      <c r="Z10" s="196"/>
+      <c r="AA10" s="197"/>
+      <c r="AB10" s="197"/>
+      <c r="AC10" s="197"/>
+      <c r="AD10" s="197"/>
+      <c r="AE10" s="197"/>
+      <c r="AF10" s="197"/>
+      <c r="AG10" s="198"/>
+      <c r="AH10" s="191" t="s">
         <v>56</v>
       </c>
-      <c r="AI10" s="171"/>
-      <c r="AJ10" s="153"/>
+      <c r="AI10" s="192"/>
+      <c r="AJ10" s="209"/>
       <c r="AK10" s="15"/>
       <c r="AL10" s="16"/>
     </row>
     <row r="11" spans="1:39" ht="27.75" customHeight="1" thickBot="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="142"/>
-      <c r="E11" s="134"/>
-      <c r="F11" s="135"/>
+      <c r="C11" s="216"/>
+      <c r="D11" s="199"/>
+      <c r="E11" s="239"/>
+      <c r="F11" s="240"/>
       <c r="G11" s="85"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="143"/>
-      <c r="L11" s="144"/>
-      <c r="M11" s="145"/>
+      <c r="K11" s="200"/>
+      <c r="L11" s="201"/>
+      <c r="M11" s="202"/>
       <c r="N11" s="19"/>
       <c r="O11" s="20"/>
       <c r="P11" s="20"/>
@@ -4676,10 +4675,10 @@
       <c r="W11" s="20"/>
       <c r="X11" s="20"/>
       <c r="Y11" s="21"/>
-      <c r="Z11" s="192" t="s">
+      <c r="Z11" s="157" t="s">
         <v>54</v>
       </c>
-      <c r="AA11" s="193"/>
+      <c r="AA11" s="158"/>
       <c r="AB11" s="22"/>
       <c r="AC11" s="22" t="s">
         <v>32</v>
@@ -4696,177 +4695,177 @@
         <v>34</v>
       </c>
       <c r="AI11" s="25"/>
-      <c r="AJ11" s="153"/>
+      <c r="AJ11" s="209"/>
       <c r="AK11" s="15"/>
       <c r="AL11" s="16"/>
     </row>
     <row r="12" spans="1:39" ht="12" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="96"/>
-      <c r="D12" s="142"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="228"/>
-      <c r="G12" s="177"/>
-      <c r="H12" s="177"/>
-      <c r="I12" s="177"/>
-      <c r="J12" s="163"/>
-      <c r="K12" s="146"/>
-      <c r="L12" s="147"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="98"/>
-      <c r="O12" s="233"/>
-      <c r="P12" s="165"/>
-      <c r="Q12" s="161"/>
-      <c r="R12" s="165"/>
-      <c r="S12" s="233"/>
-      <c r="T12" s="165"/>
-      <c r="U12" s="161"/>
-      <c r="V12" s="165"/>
-      <c r="W12" s="177"/>
-      <c r="X12" s="177"/>
-      <c r="Y12" s="163"/>
-      <c r="Z12" s="194"/>
-      <c r="AA12" s="195"/>
-      <c r="AB12" s="179"/>
-      <c r="AC12" s="181"/>
-      <c r="AD12" s="179"/>
-      <c r="AE12" s="181"/>
-      <c r="AF12" s="179"/>
-      <c r="AG12" s="163"/>
+      <c r="C12" s="216"/>
+      <c r="D12" s="199"/>
+      <c r="E12" s="185"/>
+      <c r="F12" s="187"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="136"/>
+      <c r="K12" s="203"/>
+      <c r="L12" s="148"/>
+      <c r="M12" s="204"/>
+      <c r="N12" s="185"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="116"/>
+      <c r="Q12" s="145"/>
+      <c r="R12" s="116"/>
+      <c r="S12" s="92"/>
+      <c r="T12" s="116"/>
+      <c r="U12" s="145"/>
+      <c r="V12" s="116"/>
+      <c r="W12" s="90"/>
+      <c r="X12" s="90"/>
+      <c r="Y12" s="136"/>
+      <c r="Z12" s="159"/>
+      <c r="AA12" s="160"/>
+      <c r="AB12" s="138"/>
+      <c r="AC12" s="140"/>
+      <c r="AD12" s="138"/>
+      <c r="AE12" s="140"/>
+      <c r="AF12" s="138"/>
+      <c r="AG12" s="136"/>
       <c r="AH12" s="26" t="s">
         <v>35</v>
       </c>
       <c r="AI12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AJ12" s="153"/>
+      <c r="AJ12" s="209"/>
       <c r="AK12" s="15"/>
       <c r="AL12" s="16"/>
     </row>
     <row r="13" spans="1:39" ht="12" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="142"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="177"/>
-      <c r="G13" s="177"/>
-      <c r="H13" s="177"/>
-      <c r="I13" s="177"/>
-      <c r="J13" s="163"/>
-      <c r="K13" s="146"/>
-      <c r="L13" s="147"/>
-      <c r="M13" s="148"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="233"/>
-      <c r="P13" s="165"/>
-      <c r="Q13" s="161"/>
-      <c r="R13" s="165"/>
-      <c r="S13" s="233"/>
-      <c r="T13" s="165"/>
-      <c r="U13" s="161"/>
-      <c r="V13" s="165"/>
-      <c r="W13" s="177"/>
-      <c r="X13" s="177"/>
-      <c r="Y13" s="163"/>
-      <c r="Z13" s="194"/>
-      <c r="AA13" s="195"/>
-      <c r="AB13" s="179"/>
-      <c r="AC13" s="181"/>
-      <c r="AD13" s="179"/>
-      <c r="AE13" s="181"/>
-      <c r="AF13" s="179"/>
-      <c r="AG13" s="163"/>
+      <c r="C13" s="216"/>
+      <c r="D13" s="199"/>
+      <c r="E13" s="185"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="136"/>
+      <c r="K13" s="203"/>
+      <c r="L13" s="148"/>
+      <c r="M13" s="204"/>
+      <c r="N13" s="185"/>
+      <c r="O13" s="92"/>
+      <c r="P13" s="116"/>
+      <c r="Q13" s="145"/>
+      <c r="R13" s="116"/>
+      <c r="S13" s="92"/>
+      <c r="T13" s="116"/>
+      <c r="U13" s="145"/>
+      <c r="V13" s="116"/>
+      <c r="W13" s="90"/>
+      <c r="X13" s="90"/>
+      <c r="Y13" s="136"/>
+      <c r="Z13" s="159"/>
+      <c r="AA13" s="160"/>
+      <c r="AB13" s="138"/>
+      <c r="AC13" s="140"/>
+      <c r="AD13" s="138"/>
+      <c r="AE13" s="140"/>
+      <c r="AF13" s="138"/>
+      <c r="AG13" s="136"/>
       <c r="AH13" s="26" t="s">
         <v>37</v>
       </c>
       <c r="AI13" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="AJ13" s="153"/>
+      <c r="AJ13" s="209"/>
       <c r="AK13" s="15"/>
       <c r="AL13" s="16"/>
     </row>
     <row r="14" spans="1:39" ht="12" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="142"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="177"/>
-      <c r="G14" s="177"/>
-      <c r="H14" s="177"/>
-      <c r="I14" s="177"/>
-      <c r="J14" s="163"/>
-      <c r="K14" s="146"/>
-      <c r="L14" s="147"/>
-      <c r="M14" s="148"/>
-      <c r="N14" s="98"/>
-      <c r="O14" s="233"/>
-      <c r="P14" s="165"/>
-      <c r="Q14" s="161"/>
-      <c r="R14" s="165"/>
-      <c r="S14" s="233"/>
-      <c r="T14" s="165"/>
-      <c r="U14" s="161"/>
-      <c r="V14" s="165"/>
-      <c r="W14" s="177"/>
-      <c r="X14" s="177"/>
-      <c r="Y14" s="163"/>
-      <c r="Z14" s="194"/>
-      <c r="AA14" s="195"/>
-      <c r="AB14" s="179"/>
-      <c r="AC14" s="181"/>
-      <c r="AD14" s="179"/>
-      <c r="AE14" s="181"/>
-      <c r="AF14" s="179"/>
-      <c r="AG14" s="163"/>
+      <c r="C14" s="216"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="185"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="136"/>
+      <c r="K14" s="203"/>
+      <c r="L14" s="148"/>
+      <c r="M14" s="204"/>
+      <c r="N14" s="185"/>
+      <c r="O14" s="92"/>
+      <c r="P14" s="116"/>
+      <c r="Q14" s="145"/>
+      <c r="R14" s="116"/>
+      <c r="S14" s="92"/>
+      <c r="T14" s="116"/>
+      <c r="U14" s="145"/>
+      <c r="V14" s="116"/>
+      <c r="W14" s="90"/>
+      <c r="X14" s="90"/>
+      <c r="Y14" s="136"/>
+      <c r="Z14" s="159"/>
+      <c r="AA14" s="160"/>
+      <c r="AB14" s="138"/>
+      <c r="AC14" s="140"/>
+      <c r="AD14" s="138"/>
+      <c r="AE14" s="140"/>
+      <c r="AF14" s="138"/>
+      <c r="AG14" s="136"/>
       <c r="AH14" s="26"/>
       <c r="AI14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="AJ14" s="153"/>
+      <c r="AJ14" s="209"/>
       <c r="AK14" s="15"/>
       <c r="AL14" s="16"/>
     </row>
     <row r="15" spans="1:39" ht="9" customHeight="1" thickBot="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="96"/>
-      <c r="D15" s="142"/>
-      <c r="E15" s="99"/>
-      <c r="F15" s="178"/>
-      <c r="G15" s="178"/>
-      <c r="H15" s="178"/>
-      <c r="I15" s="178"/>
-      <c r="J15" s="164"/>
-      <c r="K15" s="149"/>
-      <c r="L15" s="150"/>
-      <c r="M15" s="151"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="234"/>
-      <c r="P15" s="166"/>
-      <c r="Q15" s="162"/>
-      <c r="R15" s="166"/>
-      <c r="S15" s="234"/>
-      <c r="T15" s="166"/>
-      <c r="U15" s="162"/>
-      <c r="V15" s="166"/>
-      <c r="W15" s="178"/>
-      <c r="X15" s="178"/>
-      <c r="Y15" s="164"/>
-      <c r="Z15" s="196"/>
-      <c r="AA15" s="197"/>
-      <c r="AB15" s="180"/>
-      <c r="AC15" s="182"/>
-      <c r="AD15" s="180"/>
-      <c r="AE15" s="182"/>
-      <c r="AF15" s="180"/>
-      <c r="AG15" s="164"/>
+      <c r="C15" s="216"/>
+      <c r="D15" s="199"/>
+      <c r="E15" s="186"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="205"/>
+      <c r="L15" s="206"/>
+      <c r="M15" s="207"/>
+      <c r="N15" s="186"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="117"/>
+      <c r="Q15" s="146"/>
+      <c r="R15" s="117"/>
+      <c r="S15" s="93"/>
+      <c r="T15" s="117"/>
+      <c r="U15" s="146"/>
+      <c r="V15" s="117"/>
+      <c r="W15" s="91"/>
+      <c r="X15" s="91"/>
+      <c r="Y15" s="137"/>
+      <c r="Z15" s="161"/>
+      <c r="AA15" s="162"/>
+      <c r="AB15" s="139"/>
+      <c r="AC15" s="141"/>
+      <c r="AD15" s="139"/>
+      <c r="AE15" s="141"/>
+      <c r="AF15" s="139"/>
+      <c r="AG15" s="137"/>
       <c r="AH15" s="28"/>
       <c r="AI15" s="29"/>
-      <c r="AJ15" s="154"/>
+      <c r="AJ15" s="210"/>
       <c r="AK15" s="15"/>
       <c r="AL15" s="16"/>
       <c r="AM15" s="30"/>
@@ -4874,54 +4873,54 @@
     <row r="16" spans="1:39" ht="11.25" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="96"/>
-      <c r="D16" s="142"/>
+      <c r="C16" s="216"/>
+      <c r="D16" s="199"/>
       <c r="E16" s="84"/>
       <c r="F16" s="31"/>
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
-      <c r="J16" s="158" t="s">
+      <c r="J16" s="211" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="125"/>
-      <c r="L16" s="126"/>
-      <c r="M16" s="159" t="s">
+      <c r="K16" s="212"/>
+      <c r="L16" s="213"/>
+      <c r="M16" s="214" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="125"/>
-      <c r="O16" s="125"/>
-      <c r="P16" s="160"/>
-      <c r="Q16" s="241" t="s">
+      <c r="N16" s="212"/>
+      <c r="O16" s="212"/>
+      <c r="P16" s="215"/>
+      <c r="Q16" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="R16" s="242"/>
-      <c r="S16" s="242"/>
-      <c r="T16" s="243"/>
-      <c r="U16" s="124" t="s">
+      <c r="R16" s="102"/>
+      <c r="S16" s="102"/>
+      <c r="T16" s="103"/>
+      <c r="U16" s="237" t="s">
         <v>42</v>
       </c>
-      <c r="V16" s="125"/>
-      <c r="W16" s="125"/>
-      <c r="X16" s="125"/>
-      <c r="Y16" s="126"/>
-      <c r="Z16" s="216" t="s">
+      <c r="V16" s="212"/>
+      <c r="W16" s="212"/>
+      <c r="X16" s="212"/>
+      <c r="Y16" s="213"/>
+      <c r="Z16" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="AA16" s="217"/>
-      <c r="AB16" s="217"/>
-      <c r="AC16" s="218"/>
-      <c r="AD16" s="210" t="s">
+      <c r="AA16" s="134"/>
+      <c r="AB16" s="134"/>
+      <c r="AC16" s="135"/>
+      <c r="AD16" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="AE16" s="211"/>
-      <c r="AF16" s="211"/>
-      <c r="AG16" s="175"/>
-      <c r="AH16" s="206" t="s">
+      <c r="AE16" s="128"/>
+      <c r="AF16" s="128"/>
+      <c r="AG16" s="143"/>
+      <c r="AH16" s="171" t="s">
         <v>58</v>
       </c>
-      <c r="AI16" s="206"/>
-      <c r="AJ16" s="207"/>
+      <c r="AI16" s="171"/>
+      <c r="AJ16" s="172"/>
       <c r="AK16" s="15"/>
       <c r="AL16" s="16"/>
       <c r="AM16" s="30"/>
@@ -4929,8 +4928,8 @@
     <row r="17" spans="1:39" ht="27.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="142"/>
+      <c r="C17" s="216"/>
+      <c r="D17" s="199"/>
       <c r="E17" s="32" t="s">
         <v>43</v>
       </c>
@@ -4938,123 +4937,123 @@
       <c r="G17" s="33"/>
       <c r="H17" s="33"/>
       <c r="I17" s="34"/>
-      <c r="J17" s="113"/>
-      <c r="K17" s="114"/>
-      <c r="L17" s="115"/>
-      <c r="M17" s="110"/>
-      <c r="N17" s="111"/>
-      <c r="O17" s="111"/>
-      <c r="P17" s="112"/>
-      <c r="Q17" s="244"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="105"/>
-      <c r="U17" s="188"/>
-      <c r="V17" s="147"/>
-      <c r="W17" s="147"/>
-      <c r="X17" s="147"/>
-      <c r="Y17" s="189"/>
-      <c r="Z17" s="183"/>
-      <c r="AA17" s="147"/>
-      <c r="AB17" s="147"/>
-      <c r="AC17" s="184"/>
-      <c r="AD17" s="212"/>
-      <c r="AE17" s="213"/>
-      <c r="AF17" s="213"/>
-      <c r="AG17" s="176"/>
-      <c r="AH17" s="208"/>
-      <c r="AI17" s="208"/>
-      <c r="AJ17" s="209"/>
+      <c r="J17" s="228"/>
+      <c r="K17" s="229"/>
+      <c r="L17" s="230"/>
+      <c r="M17" s="225"/>
+      <c r="N17" s="226"/>
+      <c r="O17" s="226"/>
+      <c r="P17" s="227"/>
+      <c r="Q17" s="104"/>
+      <c r="R17" s="105"/>
+      <c r="S17" s="105"/>
+      <c r="T17" s="106"/>
+      <c r="U17" s="153"/>
+      <c r="V17" s="148"/>
+      <c r="W17" s="148"/>
+      <c r="X17" s="148"/>
+      <c r="Y17" s="154"/>
+      <c r="Z17" s="147"/>
+      <c r="AA17" s="148"/>
+      <c r="AB17" s="148"/>
+      <c r="AC17" s="149"/>
+      <c r="AD17" s="129"/>
+      <c r="AE17" s="130"/>
+      <c r="AF17" s="130"/>
+      <c r="AG17" s="144"/>
+      <c r="AH17" s="173"/>
+      <c r="AI17" s="173"/>
+      <c r="AJ17" s="174"/>
       <c r="AK17" s="35"/>
       <c r="AL17" s="16"/>
     </row>
     <row r="18" spans="1:39" ht="11.25" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="142"/>
+      <c r="C18" s="216"/>
+      <c r="D18" s="199"/>
       <c r="E18" s="36"/>
-      <c r="F18" s="119" t="s">
+      <c r="F18" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="119"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="121" t="s">
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="233"/>
+      <c r="J18" s="234" t="s">
         <v>44</v>
       </c>
-      <c r="K18" s="122"/>
-      <c r="L18" s="123"/>
-      <c r="M18" s="248"/>
-      <c r="N18" s="249"/>
-      <c r="O18" s="249"/>
-      <c r="P18" s="250"/>
-      <c r="Q18" s="244"/>
-      <c r="R18" s="104"/>
-      <c r="S18" s="104"/>
-      <c r="T18" s="105"/>
-      <c r="U18" s="188"/>
-      <c r="V18" s="147"/>
-      <c r="W18" s="147"/>
-      <c r="X18" s="147"/>
-      <c r="Y18" s="189"/>
-      <c r="Z18" s="183"/>
-      <c r="AA18" s="147"/>
-      <c r="AB18" s="147"/>
-      <c r="AC18" s="184"/>
-      <c r="AD18" s="202" t="s">
+      <c r="K18" s="235"/>
+      <c r="L18" s="236"/>
+      <c r="M18" s="113"/>
+      <c r="N18" s="114"/>
+      <c r="O18" s="114"/>
+      <c r="P18" s="115"/>
+      <c r="Q18" s="104"/>
+      <c r="R18" s="105"/>
+      <c r="S18" s="105"/>
+      <c r="T18" s="106"/>
+      <c r="U18" s="153"/>
+      <c r="V18" s="148"/>
+      <c r="W18" s="148"/>
+      <c r="X18" s="148"/>
+      <c r="Y18" s="154"/>
+      <c r="Z18" s="147"/>
+      <c r="AA18" s="148"/>
+      <c r="AB18" s="148"/>
+      <c r="AC18" s="149"/>
+      <c r="AD18" s="167" t="s">
         <v>45</v>
       </c>
-      <c r="AE18" s="204" t="s">
+      <c r="AE18" s="169" t="s">
         <v>22</v>
       </c>
-      <c r="AF18" s="214" t="s">
+      <c r="AF18" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="AG18" s="176"/>
-      <c r="AH18" s="198"/>
-      <c r="AI18" s="198"/>
-      <c r="AJ18" s="199"/>
+      <c r="AG18" s="144"/>
+      <c r="AH18" s="163"/>
+      <c r="AI18" s="163"/>
+      <c r="AJ18" s="164"/>
       <c r="AK18" s="35"/>
       <c r="AL18" s="16"/>
     </row>
     <row r="19" spans="1:39" ht="27.75" customHeight="1" thickBot="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="142"/>
+      <c r="C19" s="216"/>
+      <c r="D19" s="199"/>
       <c r="E19" s="37"/>
       <c r="F19" s="38"/>
       <c r="G19" s="38"/>
       <c r="H19" s="38"/>
       <c r="I19" s="39"/>
-      <c r="J19" s="246"/>
-      <c r="K19" s="117"/>
-      <c r="L19" s="247"/>
-      <c r="M19" s="116"/>
-      <c r="N19" s="117"/>
-      <c r="O19" s="117"/>
-      <c r="P19" s="118"/>
-      <c r="Q19" s="245"/>
-      <c r="R19" s="131"/>
-      <c r="S19" s="131"/>
-      <c r="T19" s="132"/>
-      <c r="U19" s="190"/>
-      <c r="V19" s="186"/>
-      <c r="W19" s="186"/>
-      <c r="X19" s="186"/>
-      <c r="Y19" s="191"/>
-      <c r="Z19" s="185"/>
-      <c r="AA19" s="186"/>
-      <c r="AB19" s="186"/>
-      <c r="AC19" s="187"/>
-      <c r="AD19" s="203"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="215"/>
-      <c r="AG19" s="176"/>
-      <c r="AH19" s="200"/>
-      <c r="AI19" s="200"/>
-      <c r="AJ19" s="201"/>
+      <c r="J19" s="110"/>
+      <c r="K19" s="111"/>
+      <c r="L19" s="112"/>
+      <c r="M19" s="231"/>
+      <c r="N19" s="111"/>
+      <c r="O19" s="111"/>
+      <c r="P19" s="232"/>
+      <c r="Q19" s="107"/>
+      <c r="R19" s="108"/>
+      <c r="S19" s="108"/>
+      <c r="T19" s="109"/>
+      <c r="U19" s="155"/>
+      <c r="V19" s="151"/>
+      <c r="W19" s="151"/>
+      <c r="X19" s="151"/>
+      <c r="Y19" s="156"/>
+      <c r="Z19" s="150"/>
+      <c r="AA19" s="151"/>
+      <c r="AB19" s="151"/>
+      <c r="AC19" s="152"/>
+      <c r="AD19" s="168"/>
+      <c r="AE19" s="170"/>
+      <c r="AF19" s="132"/>
+      <c r="AG19" s="144"/>
+      <c r="AH19" s="165"/>
+      <c r="AI19" s="165"/>
+      <c r="AJ19" s="166"/>
       <c r="AK19" s="15"/>
       <c r="AL19" s="16"/>
       <c r="AM19" s="40"/>
@@ -5062,8 +5061,8 @@
     <row r="20" spans="1:39" ht="33" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="96"/>
-      <c r="D20" s="142"/>
+      <c r="C20" s="216"/>
+      <c r="D20" s="199"/>
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
@@ -5080,10 +5079,10 @@
       <c r="R20" s="41"/>
       <c r="S20" s="41"/>
       <c r="T20" s="41"/>
-      <c r="U20" s="104" t="s">
+      <c r="U20" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="V20" s="104"/>
+      <c r="V20" s="105"/>
       <c r="W20" s="42"/>
       <c r="X20" s="43" t="s">
         <v>0</v>
@@ -5112,25 +5111,25 @@
     <row r="21" spans="1:39" ht="16.899999999999999" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="96"/>
-      <c r="D21" s="142"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="109"/>
-      <c r="J21" s="229" t="s">
+      <c r="C21" s="216"/>
+      <c r="D21" s="199"/>
+      <c r="E21" s="222"/>
+      <c r="F21" s="223"/>
+      <c r="G21" s="223"/>
+      <c r="H21" s="223"/>
+      <c r="I21" s="224"/>
+      <c r="J21" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="K21" s="230"/>
-      <c r="L21" s="230"/>
-      <c r="M21" s="230"/>
-      <c r="N21" s="230"/>
-      <c r="O21" s="230"/>
-      <c r="P21" s="230"/>
-      <c r="Q21" s="230"/>
-      <c r="R21" s="230"/>
-      <c r="S21" s="230"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="87"/>
+      <c r="M21" s="87"/>
+      <c r="N21" s="87"/>
+      <c r="O21" s="87"/>
+      <c r="P21" s="87"/>
+      <c r="Q21" s="87"/>
+      <c r="R21" s="87"/>
+      <c r="S21" s="87"/>
       <c r="T21" s="45"/>
       <c r="U21" s="45"/>
       <c r="V21" s="46"/>
@@ -5145,10 +5144,10 @@
       <c r="AE21" s="41"/>
       <c r="AF21" s="41"/>
       <c r="AG21" s="50"/>
-      <c r="AH21" s="174" t="s">
+      <c r="AH21" s="142" t="s">
         <v>7</v>
       </c>
-      <c r="AI21" s="174"/>
+      <c r="AI21" s="142"/>
       <c r="AJ21" s="51"/>
       <c r="AK21" s="16"/>
       <c r="AL21" s="16"/>
@@ -5156,20 +5155,20 @@
     <row r="22" spans="1:39" ht="16.899999999999999" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="142"/>
-      <c r="E22" s="235" t="s">
+      <c r="C22" s="216"/>
+      <c r="D22" s="199"/>
+      <c r="E22" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="119"/>
-      <c r="G22" s="119"/>
-      <c r="H22" s="119"/>
-      <c r="I22" s="236"/>
-      <c r="J22" s="237" t="s">
+      <c r="F22" s="95"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="97" t="s">
         <v>51</v>
       </c>
-      <c r="K22" s="238"/>
-      <c r="L22" s="238"/>
+      <c r="K22" s="98"/>
+      <c r="L22" s="98"/>
       <c r="M22" s="33"/>
       <c r="N22" s="33"/>
       <c r="O22" s="33"/>
@@ -5200,23 +5199,23 @@
     <row r="23" spans="1:39" ht="30" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="142"/>
+      <c r="C23" s="216"/>
+      <c r="D23" s="199"/>
       <c r="E23" s="55"/>
       <c r="F23" s="56"/>
       <c r="G23" s="56"/>
       <c r="H23" s="56"/>
       <c r="I23" s="57"/>
       <c r="J23" s="58"/>
-      <c r="K23" s="252"/>
-      <c r="L23" s="251"/>
-      <c r="M23" s="251"/>
-      <c r="N23" s="251"/>
-      <c r="O23" s="251"/>
-      <c r="P23" s="251"/>
-      <c r="Q23" s="251"/>
-      <c r="R23" s="251"/>
-      <c r="S23" s="251"/>
+      <c r="K23" s="251"/>
+      <c r="L23" s="252"/>
+      <c r="M23" s="252"/>
+      <c r="N23" s="252"/>
+      <c r="O23" s="252"/>
+      <c r="P23" s="252"/>
+      <c r="Q23" s="252"/>
+      <c r="R23" s="252"/>
+      <c r="S23" s="252"/>
       <c r="T23" s="83"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
@@ -5240,25 +5239,25 @@
     <row r="24" spans="1:39" ht="30" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="142"/>
-      <c r="E24" s="100" t="s">
+      <c r="C24" s="216"/>
+      <c r="D24" s="199"/>
+      <c r="E24" s="218" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="101"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="101"/>
-      <c r="I24" s="102"/>
+      <c r="F24" s="219"/>
+      <c r="G24" s="219"/>
+      <c r="H24" s="219"/>
+      <c r="I24" s="220"/>
       <c r="J24" s="61"/>
-      <c r="K24" s="239"/>
-      <c r="L24" s="240"/>
-      <c r="M24" s="240"/>
-      <c r="N24" s="240"/>
-      <c r="O24" s="240"/>
-      <c r="P24" s="240"/>
-      <c r="Q24" s="240"/>
-      <c r="R24" s="240"/>
-      <c r="S24" s="240"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="100"/>
+      <c r="M24" s="100"/>
+      <c r="N24" s="100"/>
+      <c r="O24" s="100"/>
+      <c r="P24" s="100"/>
+      <c r="Q24" s="100"/>
+      <c r="R24" s="100"/>
+      <c r="S24" s="100"/>
       <c r="T24" s="83"/>
       <c r="U24" s="62"/>
       <c r="V24" s="63"/>
@@ -5282,25 +5281,25 @@
     <row r="25" spans="1:39" ht="28.9" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="142"/>
-      <c r="E25" s="103" t="s">
+      <c r="C25" s="216"/>
+      <c r="D25" s="199"/>
+      <c r="E25" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="104"/>
-      <c r="G25" s="104"/>
-      <c r="H25" s="104"/>
-      <c r="I25" s="105"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="105"/>
+      <c r="I25" s="106"/>
       <c r="J25" s="65"/>
-      <c r="K25" s="231"/>
-      <c r="L25" s="232"/>
-      <c r="M25" s="232"/>
-      <c r="N25" s="232"/>
-      <c r="O25" s="232"/>
-      <c r="P25" s="232"/>
-      <c r="Q25" s="232"/>
-      <c r="R25" s="232"/>
-      <c r="S25" s="232"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="89"/>
+      <c r="N25" s="89"/>
+      <c r="O25" s="89"/>
+      <c r="P25" s="89"/>
+      <c r="Q25" s="89"/>
+      <c r="R25" s="89"/>
+      <c r="S25" s="89"/>
       <c r="T25" s="66"/>
       <c r="U25" s="43" t="s">
         <v>47</v>
@@ -5326,25 +5325,25 @@
     <row r="26" spans="1:39" ht="19.899999999999999" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="142"/>
+      <c r="C26" s="216"/>
+      <c r="D26" s="199"/>
       <c r="E26" s="68"/>
       <c r="F26" s="69"/>
       <c r="G26" s="69"/>
       <c r="H26" s="69"/>
       <c r="I26" s="70"/>
-      <c r="J26" s="225"/>
-      <c r="K26" s="226"/>
-      <c r="L26" s="226"/>
-      <c r="M26" s="226"/>
-      <c r="N26" s="226"/>
-      <c r="O26" s="226"/>
-      <c r="P26" s="226"/>
-      <c r="Q26" s="227"/>
-      <c r="R26" s="227"/>
-      <c r="S26" s="227"/>
-      <c r="T26" s="227"/>
-      <c r="U26" s="227"/>
+      <c r="J26" s="124"/>
+      <c r="K26" s="125"/>
+      <c r="L26" s="125"/>
+      <c r="M26" s="125"/>
+      <c r="N26" s="125"/>
+      <c r="O26" s="125"/>
+      <c r="P26" s="125"/>
+      <c r="Q26" s="126"/>
+      <c r="R26" s="126"/>
+      <c r="S26" s="126"/>
+      <c r="T26" s="126"/>
+      <c r="U26" s="126"/>
       <c r="V26" s="16"/>
       <c r="W26" s="71"/>
       <c r="X26" s="1"/>
@@ -5366,31 +5365,31 @@
     <row r="27" spans="1:39" ht="28.15" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="142"/>
-      <c r="E27" s="219" t="s">
+      <c r="C27" s="216"/>
+      <c r="D27" s="199"/>
+      <c r="E27" s="118" t="s">
         <v>53</v>
       </c>
-      <c r="F27" s="220"/>
-      <c r="G27" s="220"/>
-      <c r="H27" s="220"/>
-      <c r="I27" s="221"/>
-      <c r="J27" s="222" t="s">
+      <c r="F27" s="119"/>
+      <c r="G27" s="119"/>
+      <c r="H27" s="119"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="K27" s="223"/>
-      <c r="L27" s="223"/>
-      <c r="M27" s="223"/>
-      <c r="N27" s="223"/>
-      <c r="O27" s="223"/>
-      <c r="P27" s="223"/>
-      <c r="Q27" s="224" t="s">
+      <c r="K27" s="122"/>
+      <c r="L27" s="122"/>
+      <c r="M27" s="122"/>
+      <c r="N27" s="122"/>
+      <c r="O27" s="122"/>
+      <c r="P27" s="122"/>
+      <c r="Q27" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="R27" s="224"/>
-      <c r="S27" s="224"/>
-      <c r="T27" s="224"/>
-      <c r="U27" s="224"/>
+      <c r="R27" s="123"/>
+      <c r="S27" s="123"/>
+      <c r="T27" s="123"/>
+      <c r="U27" s="123"/>
       <c r="V27" s="73"/>
       <c r="W27" s="71"/>
       <c r="X27" s="72"/>
@@ -5411,12 +5410,12 @@
     </row>
     <row r="28" spans="1:39" ht="11.25" customHeight="1">
       <c r="X28" s="74"/>
-      <c r="Y28" s="86"/>
-      <c r="Z28" s="86"/>
-      <c r="AA28" s="86"/>
-      <c r="AB28" s="86"/>
-      <c r="AC28" s="86"/>
-      <c r="AD28" s="86"/>
+      <c r="Y28" s="241"/>
+      <c r="Z28" s="241"/>
+      <c r="AA28" s="241"/>
+      <c r="AB28" s="241"/>
+      <c r="AC28" s="241"/>
+      <c r="AD28" s="241"/>
       <c r="AE28" s="75"/>
       <c r="AF28" s="75"/>
       <c r="AG28" s="76"/>
@@ -5461,14 +5460,14 @@
       <c r="AK30" s="78"/>
     </row>
     <row r="31" spans="1:39">
-      <c r="W31" s="87" t="s">
+      <c r="W31" s="242" t="s">
         <v>49</v>
       </c>
-      <c r="X31" s="88"/>
-      <c r="Y31" s="88"/>
-      <c r="Z31" s="88"/>
-      <c r="AA31" s="88"/>
-      <c r="AB31" s="89"/>
+      <c r="X31" s="243"/>
+      <c r="Y31" s="243"/>
+      <c r="Z31" s="243"/>
+      <c r="AA31" s="243"/>
+      <c r="AB31" s="244"/>
       <c r="AD31" s="74"/>
       <c r="AE31" s="75"/>
       <c r="AF31" s="75"/>
@@ -5479,106 +5478,131 @@
       <c r="AK31" s="79"/>
     </row>
     <row r="32" spans="1:39">
-      <c r="W32" s="90" t="s">
+      <c r="W32" s="245" t="s">
         <v>48</v>
       </c>
-      <c r="X32" s="91"/>
-      <c r="Y32" s="91"/>
-      <c r="Z32" s="91"/>
-      <c r="AA32" s="91"/>
-      <c r="AB32" s="91"/>
-      <c r="AC32" s="91"/>
-      <c r="AD32" s="91"/>
-      <c r="AE32" s="91"/>
-      <c r="AF32" s="91"/>
-      <c r="AG32" s="91"/>
-      <c r="AH32" s="91"/>
-      <c r="AI32" s="91"/>
-      <c r="AJ32" s="88"/>
-      <c r="AK32" s="89"/>
+      <c r="X32" s="246"/>
+      <c r="Y32" s="246"/>
+      <c r="Z32" s="246"/>
+      <c r="AA32" s="246"/>
+      <c r="AB32" s="246"/>
+      <c r="AC32" s="246"/>
+      <c r="AD32" s="246"/>
+      <c r="AE32" s="246"/>
+      <c r="AF32" s="246"/>
+      <c r="AG32" s="246"/>
+      <c r="AH32" s="246"/>
+      <c r="AI32" s="246"/>
+      <c r="AJ32" s="243"/>
+      <c r="AK32" s="244"/>
     </row>
     <row r="33" spans="23:37">
       <c r="W33" s="80"/>
       <c r="X33" s="74"/>
-      <c r="Y33" s="92"/>
-      <c r="Z33" s="92"/>
-      <c r="AA33" s="92"/>
-      <c r="AB33" s="92"/>
-      <c r="AC33" s="92"/>
-      <c r="AD33" s="92"/>
-      <c r="AE33" s="92"/>
-      <c r="AF33" s="92"/>
-      <c r="AG33" s="92"/>
-      <c r="AH33" s="92"/>
-      <c r="AI33" s="92"/>
-      <c r="AJ33" s="92" t="s">
+      <c r="Y33" s="247"/>
+      <c r="Z33" s="247"/>
+      <c r="AA33" s="247"/>
+      <c r="AB33" s="247"/>
+      <c r="AC33" s="247"/>
+      <c r="AD33" s="247"/>
+      <c r="AE33" s="247"/>
+      <c r="AF33" s="247"/>
+      <c r="AG33" s="247"/>
+      <c r="AH33" s="247"/>
+      <c r="AI33" s="247"/>
+      <c r="AJ33" s="247" t="s">
         <v>28</v>
       </c>
-      <c r="AK33" s="93"/>
+      <c r="AK33" s="248"/>
     </row>
     <row r="34" spans="23:37">
       <c r="W34" s="80"/>
       <c r="X34" s="74"/>
-      <c r="Y34" s="92"/>
-      <c r="Z34" s="92"/>
-      <c r="AA34" s="92"/>
-      <c r="AB34" s="92"/>
-      <c r="AC34" s="92"/>
-      <c r="AD34" s="92"/>
-      <c r="AE34" s="92"/>
-      <c r="AF34" s="92"/>
-      <c r="AG34" s="92"/>
-      <c r="AH34" s="92"/>
-      <c r="AI34" s="92"/>
-      <c r="AJ34" s="92"/>
-      <c r="AK34" s="93"/>
+      <c r="Y34" s="247"/>
+      <c r="Z34" s="247"/>
+      <c r="AA34" s="247"/>
+      <c r="AB34" s="247"/>
+      <c r="AC34" s="247"/>
+      <c r="AD34" s="247"/>
+      <c r="AE34" s="247"/>
+      <c r="AF34" s="247"/>
+      <c r="AG34" s="247"/>
+      <c r="AH34" s="247"/>
+      <c r="AI34" s="247"/>
+      <c r="AJ34" s="247"/>
+      <c r="AK34" s="248"/>
     </row>
     <row r="35" spans="23:37">
       <c r="W35" s="81"/>
       <c r="X35" s="82"/>
-      <c r="Y35" s="94"/>
-      <c r="Z35" s="94"/>
-      <c r="AA35" s="94"/>
-      <c r="AB35" s="94"/>
-      <c r="AC35" s="94"/>
-      <c r="AD35" s="94"/>
-      <c r="AE35" s="94"/>
-      <c r="AF35" s="94"/>
-      <c r="AG35" s="94"/>
-      <c r="AH35" s="94"/>
-      <c r="AI35" s="94"/>
-      <c r="AJ35" s="94"/>
-      <c r="AK35" s="95"/>
+      <c r="Y35" s="249"/>
+      <c r="Z35" s="249"/>
+      <c r="AA35" s="249"/>
+      <c r="AB35" s="249"/>
+      <c r="AC35" s="249"/>
+      <c r="AD35" s="249"/>
+      <c r="AE35" s="249"/>
+      <c r="AF35" s="249"/>
+      <c r="AG35" s="249"/>
+      <c r="AH35" s="249"/>
+      <c r="AI35" s="249"/>
+      <c r="AJ35" s="249"/>
+      <c r="AK35" s="250"/>
     </row>
     <row r="37" spans="23:37" ht="84.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="K25:S25"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="O12:O15"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="K24:S24"/>
-    <mergeCell ref="K23:S23"/>
-    <mergeCell ref="Q16:T19"/>
-    <mergeCell ref="S12:S15"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="J27:P27"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="J26:P26"/>
-    <mergeCell ref="Q26:U26"/>
-    <mergeCell ref="AD16:AF17"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="Z16:AC16"/>
-    <mergeCell ref="AG12:AG15"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AC12:AC15"/>
-    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="Y28:AD28"/>
+    <mergeCell ref="W31:AB31"/>
+    <mergeCell ref="W32:AI32"/>
+    <mergeCell ref="AJ32:AK35"/>
+    <mergeCell ref="Y33:AI35"/>
+    <mergeCell ref="C8:C27"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="M5:U6"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="U16:Y16"/>
+    <mergeCell ref="Y5:AA6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="AH3:AJ4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="D8:D27"/>
+    <mergeCell ref="K11:M15"/>
+    <mergeCell ref="AJ8:AJ15"/>
+    <mergeCell ref="K8:M10"/>
+    <mergeCell ref="N8:Y10"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="Q12:Q15"/>
+    <mergeCell ref="Y12:Y15"/>
+    <mergeCell ref="T12:T15"/>
+    <mergeCell ref="R12:R15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="AL5:AL6"/>
+    <mergeCell ref="AH9:AI9"/>
+    <mergeCell ref="AH10:AI10"/>
+    <mergeCell ref="AB5:AD6"/>
+    <mergeCell ref="AE5:AG6"/>
+    <mergeCell ref="AH5:AJ6"/>
+    <mergeCell ref="AH8:AI8"/>
+    <mergeCell ref="Z8:AG10"/>
+    <mergeCell ref="E8:J10"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
     <mergeCell ref="AH21:AI21"/>
     <mergeCell ref="U20:V20"/>
     <mergeCell ref="AG16:AG19"/>
@@ -5595,58 +5619,33 @@
     <mergeCell ref="AD18:AD19"/>
     <mergeCell ref="AE18:AE19"/>
     <mergeCell ref="AH16:AJ17"/>
+    <mergeCell ref="AD16:AF17"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="Z16:AC16"/>
+    <mergeCell ref="AG12:AG15"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AC12:AC15"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="J27:P27"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="Q26:U26"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="K25:S25"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="O12:O15"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="K24:S24"/>
+    <mergeCell ref="K23:S23"/>
+    <mergeCell ref="Q16:T19"/>
+    <mergeCell ref="S12:S15"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M18:P18"/>
     <mergeCell ref="P12:P15"/>
-    <mergeCell ref="E8:J10"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="AL5:AL6"/>
-    <mergeCell ref="AH9:AI9"/>
-    <mergeCell ref="AH10:AI10"/>
-    <mergeCell ref="AB5:AD6"/>
-    <mergeCell ref="AE5:AG6"/>
-    <mergeCell ref="AH5:AJ6"/>
-    <mergeCell ref="AH8:AI8"/>
-    <mergeCell ref="Z8:AG10"/>
-    <mergeCell ref="AH3:AJ4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="D8:D27"/>
-    <mergeCell ref="K11:M15"/>
-    <mergeCell ref="AJ8:AJ15"/>
-    <mergeCell ref="K8:M10"/>
-    <mergeCell ref="N8:Y10"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="Q12:Q15"/>
-    <mergeCell ref="Y12:Y15"/>
-    <mergeCell ref="T12:T15"/>
-    <mergeCell ref="R12:R15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="C8:C27"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="M5:U6"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="U16:Y16"/>
-    <mergeCell ref="Y5:AA6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="Y28:AD28"/>
-    <mergeCell ref="W31:AB31"/>
-    <mergeCell ref="W32:AI32"/>
-    <mergeCell ref="AJ32:AK35"/>
-    <mergeCell ref="Y33:AI35"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>